<commit_message>
Added changes to .xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
   <si>
     <t>Group</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Base</t>
   </si>
   <si>
-    <t>USAG_INVPLTFRM_SYNC</t>
+    <t>USAG_LOCATION_SYNC</t>
   </si>
   <si>
     <t>V_D_DC_RLUP</t>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>BU_NUM</t>
-  </si>
-  <si>
-    <t>USAG_LOCATION_SYNC</t>
   </si>
   <si>
     <t>DC_ABBR_CD</t>
@@ -506,16 +503,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>16</v>
@@ -535,16 +532,16 @@
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>16</v>
@@ -561,19 +558,19 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>16</v>
@@ -585,10 +582,10 @@
         <v>18</v>
       </c>
       <c r="J5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -596,19 +593,19 @@
         <v>3.0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>16</v>
@@ -620,10 +617,10 @@
         <v>18</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -634,10 +631,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>14</v>
@@ -655,10 +652,10 @@
         <v>18</v>
       </c>
       <c r="J7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -669,16 +666,16 @@
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>16</v>
@@ -690,10 +687,10 @@
         <v>18</v>
       </c>
       <c r="J8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -704,16 +701,16 @@
         <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>16</v>
@@ -725,10 +722,10 @@
         <v>18</v>
       </c>
       <c r="J9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>